<commit_message>
prawie wypelniona analiza lingwistyczna
</commit_message>
<xml_diff>
--- a/DOC/Zeszyt1.xlsx
+++ b/DOC/Zeszyt1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piran\Desktop\MPSI\GIT wersjonowanie\MPSI\DOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC6815E-3190-4F78-A72A-5F021704DA4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36F715E-8FAC-4E9F-8783-86BAADA9F1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5B4330A2-7456-4F98-A0D7-2D1DFD17BCEC}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="126">
   <si>
     <t xml:space="preserve">Pracownik działu obsługi klienta </t>
   </si>
@@ -35,9 +35,6 @@
     <t xml:space="preserve">klienta </t>
   </si>
   <si>
-    <t>klient</t>
-  </si>
-  <si>
     <t xml:space="preserve">papierową kartę wniosku kredytowego </t>
   </si>
   <si>
@@ -59,9 +56,6 @@
     <t xml:space="preserve">czas spłaty </t>
   </si>
   <si>
-    <t>wniosek kredytowy</t>
-  </si>
-  <si>
     <t>dane osobowe</t>
   </si>
   <si>
@@ -92,9 +86,6 @@
     <t xml:space="preserve">zaświadczenia o dochodach klienta </t>
   </si>
   <si>
-    <t xml:space="preserve">teczce wniosku </t>
-  </si>
-  <si>
     <t>numer PESEL</t>
   </si>
   <si>
@@ -104,9 +95,6 @@
     <t>analitykowi</t>
   </si>
   <si>
-    <t>analityk</t>
-  </si>
-  <si>
     <t xml:space="preserve">Biura Informacji Kredytowej </t>
   </si>
   <si>
@@ -140,9 +128,6 @@
     <t>dzienne raporty dotyczące podejrzanych transakcji</t>
   </si>
   <si>
-    <t xml:space="preserve">Dyrektor </t>
-  </si>
-  <si>
     <t>dodatkowe parametry do przygotowania skorygowanego raportu</t>
   </si>
   <si>
@@ -197,24 +182,9 @@
     <t>[klient] wziąć [kredyty]</t>
   </si>
   <si>
-    <t>[teczka] przekazywana [analitykowi]</t>
-  </si>
-  <si>
     <t>[dzienny raport] sprawozdanie z działalności banku</t>
   </si>
   <si>
-    <t>teczkę wniosku kredytowego</t>
-  </si>
-  <si>
-    <t>opinię [analityka]</t>
-  </si>
-  <si>
-    <t>[pracownik] uzupełnia dane o kredycie</t>
-  </si>
-  <si>
-    <t>[pracownik] uzupełnia dane [adresowe klienta]</t>
-  </si>
-  <si>
     <t>[pracownik] uzupełnia dane [osobowe klienta]</t>
   </si>
   <si>
@@ -236,9 +206,6 @@
     <t>[analityk] tworzy [raport z malwersacji finansowej]</t>
   </si>
   <si>
-    <t>[analityk] wykrywa [malwersacje finansowe]</t>
-  </si>
-  <si>
     <t>[analityk] przekazuje [raport dyrektorowi]</t>
   </si>
   <si>
@@ -278,9 +245,6 @@
     <t>[dyrektor] zatwierdza [raport]</t>
   </si>
   <si>
-    <t>[dyrektor] wysyła [raport do KNF]</t>
-  </si>
-  <si>
     <t>przechowywanie [danych o klientach banku]</t>
   </si>
   <si>
@@ -291,6 +255,156 @@
   </si>
   <si>
     <t>przechowywanie [raportów dziennych z działalności banku]</t>
+  </si>
+  <si>
+    <t>Kredyt</t>
+  </si>
+  <si>
+    <t>Komisja Nadzoru Finansowego</t>
+  </si>
+  <si>
+    <t>Dyrektor</t>
+  </si>
+  <si>
+    <t>decyzja kredytowa</t>
+  </si>
+  <si>
+    <t>Klient</t>
+  </si>
+  <si>
+    <t>PESEL</t>
+  </si>
+  <si>
+    <t>Analityk</t>
+  </si>
+  <si>
+    <t>Umowa kredytowa</t>
+  </si>
+  <si>
+    <t>Raport dzienny z podejrzanych transakcji</t>
+  </si>
+  <si>
+    <t>Raport dzienny z działalności banku</t>
+  </si>
+  <si>
+    <t>Sytuacja finansowa klienta</t>
+  </si>
+  <si>
+    <t>Biuro Informacji Kredytowej</t>
+  </si>
+  <si>
+    <t>historia kredytowa</t>
+  </si>
+  <si>
+    <t>zadłużenie</t>
+  </si>
+  <si>
+    <t>Scoring Kredytowy</t>
+  </si>
+  <si>
+    <t>Opinia analityczna</t>
+  </si>
+  <si>
+    <t>raport malwersacji finansowych</t>
+  </si>
+  <si>
+    <t>status wniosku</t>
+  </si>
+  <si>
+    <t>System Turbobank</t>
+  </si>
+  <si>
+    <t>Aktor</t>
+  </si>
+  <si>
+    <t>Klasa</t>
+  </si>
+  <si>
+    <t>Atrybut</t>
+  </si>
+  <si>
+    <t>Wniosek kredytowy</t>
+  </si>
+  <si>
+    <t>zajmuje się</t>
+  </si>
+  <si>
+    <t>zgłaszają się</t>
+  </si>
+  <si>
+    <t>drukuje</t>
+  </si>
+  <si>
+    <t>[pracownik] przyjmuje [klienta]</t>
+  </si>
+  <si>
+    <t>[pracownik] wpisuje dane [adresowe klienta]</t>
+  </si>
+  <si>
+    <t>[pracownik] wpisuje [dane o kredycie]</t>
+  </si>
+  <si>
+    <t>[wniosek i dokumentacja] przekazywana [analitykowi]</t>
+  </si>
+  <si>
+    <t>wysyła [raport do KNF]</t>
+  </si>
+  <si>
+    <t>automatyzacja</t>
+  </si>
+  <si>
+    <t>Automatyzacja opiniowania wniosku</t>
+  </si>
+  <si>
+    <t>automatyzacja generacji raportów dziennych</t>
+  </si>
+  <si>
+    <t>Przechowywanie danych</t>
+  </si>
+  <si>
+    <t>generuj raport podejrzanych transakcji</t>
+  </si>
+  <si>
+    <t>przechowuj informacje o wnioskach</t>
+  </si>
+  <si>
+    <t>przechowywanie raportów dzinnych z działalności banku</t>
+  </si>
+  <si>
+    <t>usprawnić</t>
+  </si>
+  <si>
+    <t>Wniosek</t>
+  </si>
+  <si>
+    <t>Raport</t>
+  </si>
+  <si>
+    <t>Wpisz dane klienta</t>
+  </si>
+  <si>
+    <t>Wpisz ocene wniosku</t>
+  </si>
+  <si>
+    <t>Wpisz dane o Kredycie</t>
+  </si>
+  <si>
+    <t>Wyślij</t>
+  </si>
+  <si>
+    <t>Odbierz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pobierz dane </t>
+  </si>
+  <si>
+    <t>wyliczenie scoringu</t>
+  </si>
+  <si>
+    <t>Opiniuje</t>
+  </si>
+  <si>
+    <t>Przejmij wniosek</t>
   </si>
 </sst>
 </file>
@@ -330,7 +444,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -338,14 +452,68 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -660,328 +828,381 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CB46A3B-CE45-439D-9168-0EECFA4EF5DB}">
-  <dimension ref="C6:D60"/>
+  <dimension ref="C4:F61"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F5" sqref="C5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="41" customWidth="1"/>
-    <col min="4" max="4" width="39.85546875" customWidth="1"/>
-    <col min="5" max="5" width="49" customWidth="1"/>
+    <col min="3" max="4" width="39.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="39.85546875" customWidth="1"/>
+    <col min="6" max="6" width="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="2" t="s">
+    <row r="4" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C6" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="5"/>
+      <c r="E8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
+    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C17" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C18" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C24" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
+      <c r="F24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C26" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
+      <c r="D26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C27" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C28" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
+      <c r="D28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C29" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
+      <c r="F29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C30" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D25" t="s">
+      <c r="F30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C31" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
+      <c r="F31" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C32" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C33" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
+      <c r="D33" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C35" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
+      <c r="F35" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C36" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
+      <c r="F36" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C37" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C38" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
+    <row r="39" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C39" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
+      <c r="E39" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C40" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E40" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C42" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
+    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C43" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
+      <c r="D43" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C44" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
+      <c r="F44" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C45" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
+      <c r="D45" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C48" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C49" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C50" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C51" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C52" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C53" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C54" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C55" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
+      <c r="D55" s="5"/>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C56" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C51" t="s">
+      <c r="D56" s="5"/>
+    </row>
+    <row r="57" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C57" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C58" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C52" t="s">
+    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C60" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D60" s="5"/>
+    </row>
+    <row r="61" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C61" s="4" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C53" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C54" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C55" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C56" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C57" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C59" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C60" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -992,183 +1213,267 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44EB3E52-959A-4292-BB65-1AE34071F94F}">
-  <dimension ref="C6:C93"/>
+  <dimension ref="C5:E98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="41" customWidth="1"/>
+    <col min="3" max="3" width="66" customWidth="1"/>
     <col min="4" max="4" width="39.85546875" customWidth="1"/>
     <col min="5" max="5" width="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="7" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+      <c r="D24" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="14" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
+      <c r="D25" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
+    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>107</v>
+      </c>
+      <c r="D35" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>107</v>
+      </c>
+      <c r="D36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
+      <c r="D37" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
+      <c r="D38" t="s">
+        <v>111</v>
+      </c>
+      <c r="E38" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>74</v>
+      </c>
+      <c r="D39" t="s">
+        <v>112</v>
+      </c>
+      <c r="E39" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C49" s="1"/>
-    </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C62" s="1"/>
-    </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C86" s="1"/>
-    </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C87" s="1"/>
-    </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C93" s="1"/>
+      <c r="D40" t="s">
+        <v>113</v>
+      </c>
+      <c r="E40" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C54" s="1"/>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C67" s="1"/>
+    </row>
+    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C91" s="1"/>
+    </row>
+    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C92" s="1"/>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C98" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
analiza lingwistyczna w excelu ogolnie gotowa
</commit_message>
<xml_diff>
--- a/DOC/Zeszyt1.xlsx
+++ b/DOC/Zeszyt1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piran\Desktop\MPSI\GIT wersjonowanie\MPSI\DOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36F715E-8FAC-4E9F-8783-86BAADA9F1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC0B547-37B3-4E1F-80B1-4D9B1AE7B098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5B4330A2-7456-4F98-A0D7-2D1DFD17BCEC}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="119">
   <si>
     <t xml:space="preserve">Pracownik działu obsługi klienta </t>
   </si>
@@ -35,9 +35,6 @@
     <t xml:space="preserve">klienta </t>
   </si>
   <si>
-    <t xml:space="preserve">papierową kartę wniosku kredytowego </t>
-  </si>
-  <si>
     <t>i [danymi] adresowymi</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
     <t>dane adresowe</t>
   </si>
   <si>
-    <t>informacje o szczegółach kredytu</t>
-  </si>
-  <si>
     <t>rodzaj dochodu</t>
   </si>
   <si>
@@ -140,36 +134,6 @@
     <t>system informatyczny</t>
   </si>
   <si>
-    <t xml:space="preserve">dane o klientach </t>
-  </si>
-  <si>
-    <t>[dane o] wnioskach [ klientów]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bazie danych systemu </t>
-  </si>
-  <si>
-    <t xml:space="preserve">e-wniosek </t>
-  </si>
-  <si>
-    <t>automatyczne obliczenia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">generowanych raportów </t>
-  </si>
-  <si>
-    <t>skorygowanych raportów dziennych</t>
-  </si>
-  <si>
-    <t>informacji o klientach banku</t>
-  </si>
-  <si>
-    <t xml:space="preserve">procesu obsługi wniosku kredytowego </t>
-  </si>
-  <si>
-    <t xml:space="preserve">raportów działalności banku </t>
-  </si>
-  <si>
     <t>dokumentach związanych z wnioskiem [kredytowym]</t>
   </si>
   <si>
@@ -218,9 +182,6 @@
     <t>[analityk] wpisuje [ocene na wniosku]</t>
   </si>
   <si>
-    <t>raportów dotyczących podejrzanych transakcji i malwesacji finansowych</t>
-  </si>
-  <si>
     <t>[pracownik obsługi klienta] przejmuje [wniosek]</t>
   </si>
   <si>
@@ -245,9 +206,6 @@
     <t>[dyrektor] zatwierdza [raport]</t>
   </si>
   <si>
-    <t>przechowywanie [danych o klientach banku]</t>
-  </si>
-  <si>
     <t>generowanie raportów [podejrzanych transakcji i z działalności banku]</t>
   </si>
   <si>
@@ -266,9 +224,6 @@
     <t>Dyrektor</t>
   </si>
   <si>
-    <t>decyzja kredytowa</t>
-  </si>
-  <si>
     <t>Klient</t>
   </si>
   <si>
@@ -278,9 +233,6 @@
     <t>Analityk</t>
   </si>
   <si>
-    <t>Umowa kredytowa</t>
-  </si>
-  <si>
     <t>Raport dzienny z podejrzanych transakcji</t>
   </si>
   <si>
@@ -299,9 +251,6 @@
     <t>zadłużenie</t>
   </si>
   <si>
-    <t>Scoring Kredytowy</t>
-  </si>
-  <si>
     <t>Opinia analityczna</t>
   </si>
   <si>
@@ -374,37 +323,67 @@
     <t>usprawnić</t>
   </si>
   <si>
-    <t>Wniosek</t>
-  </si>
-  <si>
     <t>Raport</t>
   </si>
   <si>
-    <t>Wpisz dane klienta</t>
-  </si>
-  <si>
-    <t>Wpisz ocene wniosku</t>
-  </si>
-  <si>
-    <t>Wpisz dane o Kredycie</t>
-  </si>
-  <si>
-    <t>Wyślij</t>
-  </si>
-  <si>
-    <t>Odbierz</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pobierz dane </t>
   </si>
   <si>
-    <t>wyliczenie scoringu</t>
-  </si>
-  <si>
-    <t>Opiniuje</t>
-  </si>
-  <si>
-    <t>Przejmij wniosek</t>
+    <t>scoring kredytowy</t>
+  </si>
+  <si>
+    <t>Wysyłanie</t>
+  </si>
+  <si>
+    <t>Zapisywanie danych</t>
+  </si>
+  <si>
+    <t>Sprawdzenie</t>
+  </si>
+  <si>
+    <t>Wyliczenie</t>
+  </si>
+  <si>
+    <t>Tworzenie raportu</t>
+  </si>
+  <si>
+    <t>Ocenianie</t>
+  </si>
+  <si>
+    <t>Odczytywanie danych</t>
+  </si>
+  <si>
+    <t>Odbieranie</t>
+  </si>
+  <si>
+    <t>Przyjmowanie [informacji/danych]</t>
+  </si>
+  <si>
+    <t>kartę wniosku kredytowego</t>
+  </si>
+  <si>
+    <t>oddział banku</t>
+  </si>
+  <si>
+    <t>bank</t>
+  </si>
+  <si>
+    <t>miasto</t>
+  </si>
+  <si>
+    <t>scoring BIK</t>
+  </si>
+  <si>
+    <t>Scoring BIK</t>
+  </si>
+  <si>
+    <t>Przechowywanie</t>
+  </si>
+  <si>
+    <t>Opiniowanie wniosku</t>
+  </si>
+  <si>
+    <t>Rejestracja wniosku kredytowego</t>
   </si>
 </sst>
 </file>
@@ -493,7 +472,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -514,6 +493,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -828,10 +811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CB46A3B-CE45-439D-9168-0EECFA4EF5DB}">
-  <dimension ref="C4:F61"/>
+  <dimension ref="C1:F58"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F5" sqref="C5:F5"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,78 +824,109 @@
     <col min="6" max="6" width="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="6"/>
-      <c r="D5" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>97</v>
+    <row r="1" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="6"/>
+      <c r="D1" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C2" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="F3" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>0</v>
+      <c r="C6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C7" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>80</v>
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" t="s">
-        <v>98</v>
+      <c r="F8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" t="s">
-        <v>9</v>
+      <c r="C9" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" t="s">
-        <v>76</v>
+      <c r="F12" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="5" t="s">
         <v>6</v>
       </c>
       <c r="F13" t="s">
@@ -920,7 +934,7 @@
       </c>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F14" t="s">
@@ -929,50 +943,47 @@
     </row>
     <row r="15" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" t="s">
-        <v>8</v>
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" t="s">
-        <v>86</v>
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.25">
@@ -984,226 +995,166 @@
       </c>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C22" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" t="s">
-        <v>18</v>
+      <c r="C22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C23" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C24" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24" t="s">
-        <v>81</v>
+      <c r="C24" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C25" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D25"/>
+      <c r="E25" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C26" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D26" t="s">
-        <v>82</v>
+      <c r="F26" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C27" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E27" t="s">
-        <v>91</v>
+        <v>22</v>
+      </c>
+      <c r="F27" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C28" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="F28" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C29" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F29" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F30" t="s">
-        <v>89</v>
+      <c r="D30" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C31" s="4" t="s">
-        <v>25</v>
+      <c r="C31" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="F31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="3:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C32" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C32" s="5" t="s">
         <v>27</v>
       </c>
       <c r="F32" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C33" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D33" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C35" s="4" t="s">
+      <c r="C33" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F35" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C36" s="4" t="s">
+      <c r="F33" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C34" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F36" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C35" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C36" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E36" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C37" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E37" t="s">
-        <v>83</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C38" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="39" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C38" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C39" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E39" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="40" spans="3:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C40" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E40" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="42" spans="3:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C42" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C43" s="4" t="s">
+      <c r="F39" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C40" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D40" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C44" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F44" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C45" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D45" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C48" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C49" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C50" s="4" t="s">
-        <v>39</v>
-      </c>
+      <c r="D50" s="5"/>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C51" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C52" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C53" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C54" s="4" t="s">
-        <v>43</v>
-      </c>
+      <c r="D51" s="5"/>
     </row>
     <row r="55" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C55" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="D55" s="5"/>
     </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C56" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D56" s="5"/>
-    </row>
-    <row r="57" spans="3:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C57" s="4" t="s">
-        <v>63</v>
-      </c>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C57" s="3"/>
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C58" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C60" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D60" s="5"/>
-    </row>
-    <row r="61" spans="3:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C61" s="4" t="s">
-        <v>47</v>
-      </c>
+      <c r="C58" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1216,7 +1167,7 @@
   <dimension ref="C5:E98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,242 +1177,315 @@
     <col min="5" max="5" width="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
+      <c r="E26" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>103</v>
-      </c>
-      <c r="D10" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D11" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" t="s">
         <v>105</v>
       </c>
-      <c r="D15" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
         <v>55</v>
       </c>
-      <c r="D17" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
+      <c r="D29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
         <v>56</v>
       </c>
-      <c r="D18" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
+      <c r="E31" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D25" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>106</v>
+        <v>89</v>
+      </c>
+      <c r="E33" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="D35" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="D36" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="D37" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D38" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="E38" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="D39" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="E39" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D40" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="E40" t="s">
         <v>116</v>
       </c>
     </row>
+    <row r="47" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C47" s="4"/>
+    </row>
+    <row r="48" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C48" s="4"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49" s="4"/>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C50" s="3"/>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C51" s="3"/>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C52" s="3"/>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C53" s="3"/>
+    </row>
     <row r="54" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C54" s="1"/>
+      <c r="C54" s="3"/>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C55" s="3"/>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C56" s="3"/>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C57" s="3"/>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C58" s="3"/>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C59" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C60" s="3" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C67" s="1"/>

</xml_diff>